<commit_message>
Atualização Mapeamento Conferência LN
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Conferencia_BAL.xlsx
+++ b/Documentação/Planilhas/Conferencia_BAL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" tabRatio="812" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" tabRatio="812"/>
   </bookViews>
   <sheets>
     <sheet name="stg_bal_balancete" sheetId="33" r:id="rId1"/>
@@ -195,9 +195,6 @@
     <t>68661.3400</t>
   </si>
   <si>
-    <t>ttadv3580m000</t>
-  </si>
-  <si>
     <t xml:space="preserve">Foi criada uma query para auxiliar a conferencia dos dados
 Na sessão ttadv3580m000, selecionar a consulta tfgld205b (Validação do Balancete BI). 
 Ir em Ações e selecionar  Run Query. Na sequência, clique em Executar. 
@@ -206,9 +203,6 @@
 </t>
   </si>
   <si>
-    <t>tfgld3501m000</t>
-  </si>
-  <si>
     <t>CD_CHAVE_PRIMARIA</t>
   </si>
   <si>
@@ -310,6 +304,12 @@
   </si>
   <si>
     <t>Na aba Histórico, clicar sobre o link existente no campo Tipo de Transação e pegar a informação da coluna Categoria da Transação referente ao Tipo de Transação que está sendo analisado</t>
+  </si>
+  <si>
+    <t>tfgld3501m000 (Histórico da Conta)</t>
+  </si>
+  <si>
+    <t>ttadv3580m000 (Query Data)</t>
   </si>
 </sst>
 </file>
@@ -441,23 +441,23 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -766,7 +766,9 @@
   </sheetPr>
   <dimension ref="A1:AE31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
@@ -791,10 +793,10 @@
       <c r="AE1" s="2"/>
     </row>
     <row r="2" spans="1:31" ht="21">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="15"/>
+      <c r="B2" s="17"/>
       <c r="C2" s="3" t="s">
         <v>24</v>
       </c>
@@ -803,12 +805,12 @@
       <c r="AE2" s="2"/>
     </row>
     <row r="3" spans="1:31" ht="21">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="15"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="3" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
       <c r="R3" s="2"/>
       <c r="T3" s="2"/>
@@ -1233,123 +1235,123 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="11.25" customHeight="1">
-      <c r="A19" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
+      <c r="A19" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
+      <c r="A31" s="18"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1369,7 +1371,9 @@
   </sheetPr>
   <dimension ref="A1:AF48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
@@ -1400,10 +1404,10 @@
       <c r="AF1" s="2"/>
     </row>
     <row r="2" spans="1:32" s="1" customFormat="1" ht="21">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="15"/>
+      <c r="B2" s="17"/>
       <c r="C2" s="3" t="s">
         <v>24</v>
       </c>
@@ -1421,12 +1425,12 @@
       <c r="AE2" s="2"/>
     </row>
     <row r="3" spans="1:32" s="1" customFormat="1" ht="21">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="15"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="3" t="s">
-        <v>58</v>
+        <v>90</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1442,75 +1446,75 @@
       <c r="AE3" s="2"/>
     </row>
     <row r="5" spans="1:32" s="1" customFormat="1" ht="21" customHeight="1">
-      <c r="A5" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
+      <c r="A5" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
       <c r="N5" s="2"/>
     </row>
     <row r="6" spans="1:32" s="1" customFormat="1">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
       <c r="N6" s="2"/>
     </row>
     <row r="7" spans="1:32" s="1" customFormat="1">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
       <c r="N7" s="2"/>
     </row>
     <row r="8" spans="1:32" s="1" customFormat="1">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
       <c r="N8" s="2"/>
     </row>
     <row r="9" spans="1:32" s="1" customFormat="1">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
       <c r="N9" s="2"/>
     </row>
     <row r="10" spans="1:32" s="1" customFormat="1">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
       <c r="N10" s="2"/>
     </row>
     <row r="11" spans="1:32" s="1" customFormat="1">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
       <c r="N11" s="2"/>
     </row>
     <row r="12" spans="1:32" s="1" customFormat="1">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
       <c r="N12" s="2"/>
     </row>
     <row r="13" spans="1:32" s="1" customFormat="1">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
+      <c r="A13" s="20"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
       <c r="N13" s="2"/>
     </row>
     <row r="14" spans="1:32" s="1" customFormat="1">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
       <c r="N14" s="2"/>
     </row>
     <row r="15" spans="1:32" s="1" customFormat="1">
@@ -1524,10 +1528,10 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>17</v>
@@ -1545,30 +1549,30 @@
         <v>16</v>
       </c>
       <c r="H17" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J17" s="8" t="s">
         <v>61</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>63</v>
       </c>
       <c r="K17" s="8" t="s">
         <v>21</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C18" s="10">
         <v>320101026</v>
@@ -1586,13 +1590,13 @@
         <v>201</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I18" s="10">
         <v>2</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K18" s="10">
         <v>8</v>
@@ -1606,10 +1610,10 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C19" s="10">
         <v>320101026</v>
@@ -1627,13 +1631,13 @@
         <v>201</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I19" s="10">
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K19" s="10">
         <v>1</v>
@@ -1647,10 +1651,10 @@
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C20" s="10">
         <v>320110025</v>
@@ -1668,13 +1672,13 @@
         <v>201</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I20" s="10">
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K20" s="10">
         <v>1</v>
@@ -1688,10 +1692,10 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C21" s="10">
         <v>320115003</v>
@@ -1709,7 +1713,7 @@
         <v>201</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I21" s="10">
         <v>2</v>
@@ -1737,74 +1741,74 @@
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
-      <c r="J22" s="19"/>
+      <c r="J22" s="15"/>
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
     </row>
     <row r="24" spans="1:13" ht="11.25" customHeight="1">
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="F24" s="19"/>
+      <c r="G24" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="H24" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="I24" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="E24" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16" t="s">
+      <c r="J24" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="H24" s="16" t="s">
+      <c r="K24" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="I24" s="16" t="s">
+      <c r="L24" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="J24" s="16" t="s">
+      <c r="M24" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="K24" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="L24" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="M24" s="16" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="25" spans="1:13">
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
-      <c r="L25" s="16"/>
-      <c r="M25" s="16"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
     </row>
     <row r="26" spans="1:13">
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
     </row>
     <row r="27" spans="1:13">
       <c r="B27" s="1"/>
@@ -1823,7 +1827,7 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="K28" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="123.75">
@@ -1887,33 +1891,33 @@
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
-      <c r="K37" s="20"/>
+      <c r="K37" s="16"/>
     </row>
     <row r="38" spans="2:11">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
-      <c r="K38" s="20"/>
+      <c r="K38" s="16"/>
     </row>
     <row r="39" spans="2:11">
       <c r="C39" s="1"/>
-      <c r="K39" s="20"/>
+      <c r="K39" s="16"/>
     </row>
     <row r="40" spans="2:11">
       <c r="C40" s="1"/>
-      <c r="K40" s="20"/>
+      <c r="K40" s="16"/>
     </row>
     <row r="41" spans="2:11">
       <c r="C41" s="1"/>
-      <c r="K41" s="20"/>
+      <c r="K41" s="16"/>
     </row>
     <row r="42" spans="2:11">
       <c r="C42" s="1"/>
-      <c r="K42" s="20"/>
+      <c r="K42" s="16"/>
     </row>
     <row r="43" spans="2:11">
       <c r="C43" s="1"/>
-      <c r="K43" s="20"/>
+      <c r="K43" s="16"/>
     </row>
     <row r="44" spans="2:11">
       <c r="C44" s="1"/>
@@ -1932,6 +1936,10 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
     <mergeCell ref="K24:K26"/>
     <mergeCell ref="A5:D14"/>
     <mergeCell ref="L24:L26"/>
@@ -1942,10 +1950,6 @@
     <mergeCell ref="D24:D26"/>
     <mergeCell ref="E24:F26"/>
     <mergeCell ref="G24:G26"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>